<commit_message>
modifications on the budget
</commit_message>
<xml_diff>
--- a/budget_project.xlsx
+++ b/budget_project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="1020" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
     <t>FRENCH COORDINATOR: Emmanuel Dupoux</t>
   </si>
   <si>
-    <t>15 k $</t>
+    <t xml:space="preserve">$ 15 k </t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>

</xml_diff>